<commit_message>
Adding data buoy node bill of materials
</commit_message>
<xml_diff>
--- a/gps-node/bill_of_materials.xlsx
+++ b/gps-node/bill_of_materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdmed\Downloads\Uniandes\AsistenciaInvestigacion\OpenSourceDataBuoy\open-source-fish-farming-prototypes\gps-node\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382ECEEA-E06D-4936-8F3A-F345824502DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D57765A-EBA3-4B5C-923C-CD7F4529F691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21600" xr2:uid="{CBC51B39-64A4-4F9B-B35D-416E43FC5AB9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>BILL OF MATERIALS - GPS NODE</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>PLA filament</t>
+  </si>
+  <si>
+    <t>AA Battery</t>
   </si>
 </sst>
 </file>
@@ -187,13 +190,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -509,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{753CFBDF-9549-4D5C-9A5F-E33649E0A1D6}">
-  <dimension ref="B2:D17"/>
+  <dimension ref="B2:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -523,23 +526,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="21" x14ac:dyDescent="0.5">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="2"/>
     </row>
     <row r="4" spans="2:4" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="B4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
     </row>
     <row r="6" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
@@ -613,25 +616,33 @@
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C15" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding i2c switching code
</commit_message>
<xml_diff>
--- a/gps-node/bill_of_materials.xlsx
+++ b/gps-node/bill_of_materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdmed\Downloads\Uniandes\AsistenciaInvestigacion\OpenSourceDataBuoy\open-source-fish-farming-prototypes\gps-node\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D57765A-EBA3-4B5C-923C-CD7F4529F691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B40148A-DB7E-44F1-BE5E-808AA83097C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21600" xr2:uid="{CBC51B39-64A4-4F9B-B35D-416E43FC5AB9}"/>
   </bookViews>
@@ -515,7 +515,7 @@
   <dimension ref="B2:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>